<commit_message>
Monte Carlo improvements: . Added stochastic load behavior to MC considering a bi-variate normal PDF. Constant relationship between mean and variance -> variance(t) = mean(t)/5
</commit_message>
<xml_diff>
--- a/Pyomo/MILP_v1/Input_Files/InputData34_v4congested.xlsx
+++ b/Pyomo/MILP_v1/Input_Files/InputData34_v4congested.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Forro\PycharmProjects\MasterThesis\Pyomo\MILP_v1\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228882CC-0B71-4162-B409-141CDDD53363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E91DA5-D2F7-4EC8-A512-78DCE3AC5ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11325" tabRatio="890" firstSheet="2" activeTab="2" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11325" tabRatio="890" firstSheet="6" activeTab="10" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
   </bookViews>
   <sheets>
     <sheet name="LineData" sheetId="3" r:id="rId1"/>
@@ -2388,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C888424A-DB72-4D36-91F6-3CF3A5F0E23C}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4557,7 +4557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C3061C-7501-402D-9903-D99F079214AE}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -5040,7 +5040,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5476,7 +5476,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5842,7 +5842,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5908,7 +5908,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Stochastic load fixes . affine transformation of the multivariate normal using Cholesky decomposition to obtain P and Q. The correlation needs to be normalized by variance of Q
</commit_message>
<xml_diff>
--- a/Pyomo/MILP_v1/Input_Files/InputData34_v4congested.xlsx
+++ b/Pyomo/MILP_v1/Input_Files/InputData34_v4congested.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Forro\PycharmProjects\MasterThesis\Pyomo\MILP_v1\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E91DA5-D2F7-4EC8-A512-78DCE3AC5ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72566195-AF5A-4576-8B55-B81BEFF6F93A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11325" tabRatio="890" firstSheet="6" activeTab="10" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="890" activeTab="9" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
   </bookViews>
   <sheets>
     <sheet name="LineData" sheetId="3" r:id="rId1"/>
@@ -1638,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C358DC-12EF-4E1A-B9B4-66615C268D13}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1693,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C3">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D3">
         <v>1000</v>
@@ -1735,7 +1735,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C5">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D5">
         <v>1000</v>
@@ -1756,7 +1756,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C6">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D6">
         <v>1000</v>
@@ -1819,7 +1819,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C9">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D9">
         <v>1000</v>
@@ -1840,7 +1840,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C10">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D10">
         <v>1000</v>
@@ -1882,7 +1882,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C12">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D12">
         <v>1000</v>
@@ -1903,7 +1903,7 @@
         <v>77.599999999999994</v>
       </c>
       <c r="C13">
-        <v>0.85241174791294305</v>
+        <v>0.98</v>
       </c>
       <c r="D13">
         <v>1000</v>
@@ -1924,7 +1924,7 @@
         <v>40.799999999999997</v>
       </c>
       <c r="C14">
-        <v>0.84799830400508802</v>
+        <v>0.98</v>
       </c>
       <c r="D14">
         <v>1000</v>
@@ -1945,7 +1945,7 @@
         <v>40.799999999999997</v>
       </c>
       <c r="C15">
-        <v>0.84799830400508802</v>
+        <v>0.98</v>
       </c>
       <c r="D15">
         <v>1000</v>
@@ -1966,7 +1966,7 @@
         <v>40.799999999999997</v>
       </c>
       <c r="C16">
-        <v>0.84799830400508802</v>
+        <v>0.98</v>
       </c>
       <c r="D16">
         <v>1000</v>
@@ -1987,7 +1987,7 @@
         <v>7.6</v>
       </c>
       <c r="C17">
-        <v>0.87524153543926952</v>
+        <v>0.98</v>
       </c>
       <c r="D17">
         <v>1000</v>
@@ -2008,7 +2008,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C18">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D18">
         <v>1000</v>
@@ -2029,7 +2029,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C19">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D19">
         <v>1000</v>
@@ -2050,7 +2050,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C20">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D20">
         <v>1000</v>
@@ -2071,7 +2071,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C21">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D21">
         <v>1000</v>
@@ -2092,7 +2092,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C22">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D22">
         <v>1000</v>
@@ -2113,7 +2113,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C23">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D23">
         <v>1000</v>
@@ -2134,7 +2134,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C24">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D24">
         <v>1000</v>
@@ -2155,7 +2155,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C25">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D25">
         <v>1000</v>
@@ -2176,7 +2176,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C26">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D26">
         <v>1000</v>
@@ -2197,7 +2197,7 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C27">
-        <v>0.85015388881294152</v>
+        <v>0.98</v>
       </c>
       <c r="D27">
         <v>1000</v>
@@ -2218,7 +2218,7 @@
         <v>77.599999999999994</v>
       </c>
       <c r="C28">
-        <v>0.84996155029196663</v>
+        <v>0.98</v>
       </c>
       <c r="D28">
         <v>1000</v>
@@ -2239,7 +2239,7 @@
         <v>42.5</v>
       </c>
       <c r="C29">
-        <v>0.84227140066151129</v>
+        <v>0.98</v>
       </c>
       <c r="D29">
         <v>1000</v>
@@ -2260,7 +2260,7 @@
         <v>42.5</v>
       </c>
       <c r="C30">
-        <v>0.84227140066151129</v>
+        <v>0.98</v>
       </c>
       <c r="D30">
         <v>1000</v>
@@ -2281,7 +2281,7 @@
         <v>42.5</v>
       </c>
       <c r="C31">
-        <v>0.84227140066151129</v>
+        <v>0.98</v>
       </c>
       <c r="D31">
         <v>1000</v>
@@ -2302,7 +2302,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="C32">
-        <v>0.83601080746216316</v>
+        <v>0.98</v>
       </c>
       <c r="D32">
         <v>1000</v>
@@ -2323,7 +2323,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="C33">
-        <v>0.83601080746216316</v>
+        <v>0.98</v>
       </c>
       <c r="D33">
         <v>1000</v>
@@ -2344,7 +2344,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="C34">
-        <v>0.83601080746216316</v>
+        <v>0.98</v>
       </c>
       <c r="D34">
         <v>1000</v>
@@ -2365,7 +2365,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="C35">
-        <v>0.83601080746216316</v>
+        <v>0.98</v>
       </c>
       <c r="D35">
         <v>1000</v>
@@ -2388,7 +2388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C888424A-DB72-4D36-91F6-3CF3A5F0E23C}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>

</xml_diff>